<commit_message>
adding older press releases
</commit_message>
<xml_diff>
--- a/ta/ta-sources.xlsx
+++ b/ta/ta-sources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lbc8\Desktop\GitRepos\OAlanguage\ta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lbc8\Desktop\GitRepos\OAlanguage\TA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908DF418-2930-49F4-8375-4E1A8D145B3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C182E683-33D6-4C64-9D3C-067920666C9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{0111C5F6-399B-4562-A450-E1FAE574C03C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0111C5F6-399B-4562-A450-E1FAE574C03C}"/>
   </bookViews>
   <sheets>
     <sheet name="Press Releases" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>Publisher</t>
   </si>
@@ -158,6 +158,21 @@
   </si>
   <si>
     <t>MIT</t>
+  </si>
+  <si>
+    <t>Talor and Francis</t>
+  </si>
+  <si>
+    <t>VSNU</t>
+  </si>
+  <si>
+    <t>https://www.vsnu.nl/en_GB/news-items.html/nieuwsbericht/259</t>
+  </si>
+  <si>
+    <t>tf-vsnu-16</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -509,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29BD8EB6-073A-49FA-9B2B-54D2FCC0BF92}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -522,7 +537,7 @@
     <col min="3" max="3" width="23.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,8 +550,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -549,8 +567,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -563,8 +584,11 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -577,8 +601,11 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -591,8 +618,11 @@
       <c r="D5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -605,8 +635,11 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -618,6 +651,26 @@
       </c>
       <c r="D7" t="s">
         <v>27</v>
+      </c>
+      <c r="E7">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8">
+        <v>2016</v>
       </c>
     </row>
   </sheetData>
@@ -629,7 +682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3753E9-DC89-4EC7-80A2-070DE151B247}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>